<commit_message>
Added VGG Model and Execution
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E214AE-282A-4AC6-9F9C-97F7806A77D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1294AD6E-22B1-4C5B-BA45-8C21B4D912F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="42">
   <si>
     <t>Batch Size</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>0-.15</t>
+  </si>
+  <si>
+    <t>VGGNet + LSTM</t>
+  </si>
+  <si>
+    <t>VGG16 + LSTM</t>
   </si>
 </sst>
 </file>
@@ -163,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +188,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -364,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -390,6 +402,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,6 +426,136 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -481,14 +628,16 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -502,143 +651,11 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -661,20 +678,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1C24375-E5F9-4CF2-995E-5E785518B709}" name="Table1" displayName="Table1" ref="A1:K10" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1C24375-E5F9-4CF2-995E-5E785518B709}" name="Table1" displayName="Table1" ref="A1:K10" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:K10" xr:uid="{F9E899B8-83C9-4EEB-A9DD-FACD6F61AE4A}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{40C7D022-C54A-4A02-896C-4BF0416DF703}" name="Batch Size" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{34A1F617-8830-4F5F-956C-895C47552589}" name="Image Size" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{08B576D0-877A-4B5D-8590-F007E627B83D}" name="Layers" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{D1AFC047-F699-47E3-9D75-7729D8193FE9}" name="Learning Rate" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{1FF90751-690E-4ABA-89D9-3E37230A8DDD}" name="Image Count Consdered" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{2FF43F68-2D4B-4B6F-8751-5DA818C82A13}" name="DecayLR" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{82FFDA63-E0E3-4D36-BFC3-57B6F0D81D32}" name="Accuracy After 5 Epoc" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{BBD13C41-7152-40B4-9FDD-85AE1AFBF0D0}" name="Accuracy After 10 Epoc" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{53B77158-50DC-42E0-9EA5-3E9CC2E3365B}" name="Filter" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{26795645-7AC8-4FDA-8D5F-08407EB9FA27}" name="DropOut" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{1E3A28C4-8E56-4A48-9666-69C8260765FB}" name="Alogithm" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{40C7D022-C54A-4A02-896C-4BF0416DF703}" name="Batch Size" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{34A1F617-8830-4F5F-956C-895C47552589}" name="Image Size" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{08B576D0-877A-4B5D-8590-F007E627B83D}" name="Layers" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{D1AFC047-F699-47E3-9D75-7729D8193FE9}" name="Learning Rate" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{1FF90751-690E-4ABA-89D9-3E37230A8DDD}" name="Image Count Consdered" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{2FF43F68-2D4B-4B6F-8751-5DA818C82A13}" name="DecayLR" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{82FFDA63-E0E3-4D36-BFC3-57B6F0D81D32}" name="Accuracy After 5 Epoc" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{BBD13C41-7152-40B4-9FDD-85AE1AFBF0D0}" name="Accuracy After 10 Epoc" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{53B77158-50DC-42E0-9EA5-3E9CC2E3365B}" name="Filter" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{26795645-7AC8-4FDA-8D5F-08407EB9FA27}" name="DropOut" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{1E3A28C4-8E56-4A48-9666-69C8260765FB}" name="Alogithm" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -946,7 +963,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1449,35 +1466,35 @@
       <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+      <c r="A16" s="19">
         <v>20</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="20">
         <v>0.1</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="20">
         <v>15</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="20">
         <v>0.5</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="20">
         <v>0.87</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="22">
         <v>0.87</v>
       </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="23" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1614,17 +1631,37 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="9">
+        <v>15</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0.1</v>
+      </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="12"/>
+      <c r="J21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>

</xml_diff>